<commit_message>
update styles and protocol
</commit_message>
<xml_diff>
--- a/IssueTrackingSystem/docs/JS-Frameworks-Self-Evaluation-Protocol.xlsx
+++ b/IssueTrackingSystem/docs/JS-Frameworks-Self-Evaluation-Protocol.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
   <si>
     <t>JS-SPA-Self-Evaluation-Protocol</t>
   </si>
@@ -129,9 +129,6 @@
   </si>
   <si>
     <t>-&gt;Projects</t>
-  </si>
-  <si>
-    <t>ima za doopravqne</t>
   </si>
   <si>
     <r>
@@ -162,7 +159,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -206,6 +203,15 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <i val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -281,7 +287,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -338,6 +344,18 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -347,6 +365,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -442,7 +468,7 @@
   <dimension ref="B1:E32"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="G24" activeCellId="0" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -583,31 +609,31 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="12" t="s">
+    <row r="13" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="13" t="n">
+      <c r="C13" s="16" t="n">
         <v>5</v>
       </c>
-      <c r="D13" s="13" t="n">
+      <c r="D13" s="16" t="n">
         <v>5</v>
       </c>
-      <c r="E13" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="12" t="s">
+      <c r="E13" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="13" t="n">
-        <v>10</v>
-      </c>
-      <c r="D14" s="13" t="n">
-        <v>10</v>
-      </c>
-      <c r="E14" s="13" t="s">
+      <c r="C14" s="16" t="n">
+        <v>10</v>
+      </c>
+      <c r="D14" s="16" t="n">
+        <v>10</v>
+      </c>
+      <c r="E14" s="16" t="s">
         <v>18</v>
       </c>
     </row>
@@ -663,17 +689,17 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="12" t="s">
+    <row r="19" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="13" t="n">
+      <c r="C19" s="16" t="n">
         <v>15</v>
       </c>
-      <c r="D19" s="13" t="n">
+      <c r="D19" s="16" t="n">
         <v>15</v>
       </c>
-      <c r="E19" s="13"/>
+      <c r="E19" s="16"/>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="12" t="s">
@@ -685,31 +711,31 @@
       </c>
       <c r="E20" s="13"/>
     </row>
-    <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="12" t="s">
+    <row r="21" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="13" t="n">
-        <v>10</v>
-      </c>
-      <c r="D21" s="13" t="n">
-        <v>10</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="12" t="s">
+      <c r="C21" s="16" t="n">
+        <v>10</v>
+      </c>
+      <c r="D21" s="16" t="n">
+        <v>10</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="13" t="n">
+      <c r="C22" s="16" t="n">
         <v>5</v>
       </c>
-      <c r="D22" s="13" t="n">
+      <c r="D22" s="16" t="n">
         <v>5</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="E22" s="16" t="s">
         <v>18</v>
       </c>
     </row>
@@ -724,109 +750,109 @@
       <c r="E23" s="13"/>
     </row>
     <row r="24" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="16" t="n">
+      <c r="C25" s="19" t="n">
         <v>20</v>
       </c>
-      <c r="D25" s="16" t="n">
+      <c r="D25" s="19" t="n">
         <v>20</v>
       </c>
-      <c r="E25" s="16" t="s">
+      <c r="E25" s="19" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="16" t="n">
+      <c r="C26" s="19" t="n">
         <v>20</v>
       </c>
-      <c r="D26" s="16" t="n">
+      <c r="D26" s="19" t="n">
         <v>20</v>
       </c>
-      <c r="E26" s="16" t="s">
-        <v>18</v>
+      <c r="E26" s="19" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16" t="n">
-        <v>10</v>
-      </c>
-      <c r="E28" s="16"/>
-    </row>
-    <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="15" t="s">
+      <c r="C28" s="19"/>
+      <c r="D28" s="19" t="n">
+        <v>10</v>
+      </c>
+      <c r="E28" s="19"/>
+    </row>
+    <row r="29" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="16" t="n">
-        <v>10</v>
-      </c>
-      <c r="D29" s="16" t="n">
-        <v>10</v>
-      </c>
-      <c r="E29" s="16" t="s">
+      <c r="C29" s="21" t="n">
+        <v>10</v>
+      </c>
+      <c r="D29" s="21" t="n">
+        <v>10</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="22" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="17" t="s">
+      <c r="C30" s="19" t="n">
+        <v>15</v>
+      </c>
+      <c r="D30" s="19" t="n">
+        <v>15</v>
+      </c>
+      <c r="E30" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="16" t="n">
-        <v>15</v>
-      </c>
-      <c r="D30" s="16" t="n">
-        <v>15</v>
-      </c>
-      <c r="E30" s="16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="15" t="s">
+      <c r="C31" s="19"/>
+      <c r="D31" s="19" t="n">
+        <v>5</v>
+      </c>
+      <c r="E31" s="19"/>
+    </row>
+    <row r="32" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16" t="n">
-        <v>5</v>
-      </c>
-      <c r="E31" s="16"/>
-    </row>
-    <row r="32" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" s="19" t="n">
+      <c r="C32" s="24" t="n">
         <f aca="false">SUM(C6:C31)</f>
         <v>437</v>
       </c>
-      <c r="D32" s="19" t="n">
+      <c r="D32" s="24" t="n">
         <v>330</v>
       </c>
-      <c r="E32" s="18"/>
+      <c r="E32" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
using min version for all js file and css file
</commit_message>
<xml_diff>
--- a/IssueTrackingSystem/docs/JS-Frameworks-Self-Evaluation-Protocol.xlsx
+++ b/IssueTrackingSystem/docs/JS-Frameworks-Self-Evaluation-Protocol.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
   <si>
     <t>JS-SPA-Self-Evaluation-Protocol</t>
   </si>
@@ -159,7 +159,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -213,6 +213,15 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <i val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -336,6 +345,18 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -344,18 +365,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -376,7 +385,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -468,7 +477,7 @@
   <dimension ref="B1:E32"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G24" activeCellId="0" sqref="G24"/>
+      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -550,7 +559,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="9" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>13</v>
@@ -564,7 +573,7 @@
         <v>15</v>
       </c>
       <c r="C9" s="9" t="n">
-        <v>236</v>
+        <v>266</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>13</v>
@@ -581,173 +590,173 @@
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
     </row>
-    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="12" t="s">
+    <row r="11" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="13" t="n">
+      <c r="C11" s="14" t="n">
         <v>15</v>
       </c>
-      <c r="D11" s="13" t="n">
+      <c r="D11" s="14" t="n">
         <v>20</v>
       </c>
-      <c r="E11" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="12" t="s">
+      <c r="E11" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="13" t="n">
+      <c r="C12" s="14" t="n">
         <v>25</v>
       </c>
-      <c r="D12" s="13" t="n">
+      <c r="D12" s="14" t="n">
         <v>30</v>
       </c>
-      <c r="E12" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="15" t="s">
+      <c r="E12" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="16" t="n">
+      <c r="C13" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="D13" s="16" t="n">
+      <c r="D13" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="E13" s="16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="15" t="s">
+      <c r="E13" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="16" t="n">
-        <v>10</v>
-      </c>
-      <c r="D14" s="16" t="n">
-        <v>10</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="12" t="s">
+      <c r="C14" s="14" t="n">
+        <v>10</v>
+      </c>
+      <c r="D14" s="14" t="n">
+        <v>10</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="13" t="n">
-        <v>10</v>
-      </c>
-      <c r="D15" s="13" t="n">
-        <v>10</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="12" t="s">
+      <c r="C15" s="14" t="n">
+        <v>10</v>
+      </c>
+      <c r="D15" s="14" t="n">
+        <v>10</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="13" t="n">
-        <v>10</v>
-      </c>
-      <c r="D16" s="13" t="n">
-        <v>10</v>
-      </c>
-      <c r="E16" s="13" t="s">
+      <c r="C16" s="14" t="n">
+        <v>10</v>
+      </c>
+      <c r="D16" s="14" t="n">
+        <v>10</v>
+      </c>
+      <c r="E16" s="14" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13" t="n">
+      <c r="C17" s="16"/>
+      <c r="D17" s="16" t="n">
         <v>5</v>
       </c>
-      <c r="E17" s="13"/>
+      <c r="E17" s="16"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="13" t="n">
-        <v>10</v>
-      </c>
-      <c r="D18" s="13" t="n">
-        <v>10</v>
-      </c>
-      <c r="E18" s="13" t="s">
+      <c r="C18" s="16" t="n">
+        <v>10</v>
+      </c>
+      <c r="D18" s="16" t="n">
+        <v>10</v>
+      </c>
+      <c r="E18" s="16" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="15" t="s">
+    <row r="19" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="16" t="n">
+      <c r="C19" s="14" t="n">
         <v>15</v>
       </c>
-      <c r="D19" s="16" t="n">
+      <c r="D19" s="14" t="n">
         <v>15</v>
       </c>
-      <c r="E19" s="16"/>
+      <c r="E19" s="14"/>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13" t="n">
-        <v>10</v>
-      </c>
-      <c r="E20" s="13"/>
-    </row>
-    <row r="21" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="15" t="s">
+      <c r="C20" s="16"/>
+      <c r="D20" s="16" t="n">
+        <v>10</v>
+      </c>
+      <c r="E20" s="16"/>
+    </row>
+    <row r="21" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="16" t="n">
-        <v>10</v>
-      </c>
-      <c r="D21" s="16" t="n">
-        <v>10</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="15" t="s">
+      <c r="C21" s="14" t="n">
+        <v>10</v>
+      </c>
+      <c r="D21" s="14" t="n">
+        <v>10</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="16" t="n">
+      <c r="C22" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="D22" s="16" t="n">
+      <c r="D22" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="E22" s="16" t="s">
+      <c r="E22" s="14" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13" t="n">
-        <v>10</v>
-      </c>
-      <c r="E23" s="13"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16" t="n">
+        <v>10</v>
+      </c>
+      <c r="E23" s="16"/>
     </row>
     <row r="24" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="17" t="s">
@@ -793,17 +802,21 @@
       <c r="D27" s="19"/>
       <c r="E27" s="19"/>
     </row>
-    <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="18" t="s">
+    <row r="28" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19" t="n">
-        <v>10</v>
-      </c>
-      <c r="E28" s="19"/>
-    </row>
-    <row r="29" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C28" s="21" t="n">
+        <v>10</v>
+      </c>
+      <c r="D28" s="21" t="n">
+        <v>10</v>
+      </c>
+      <c r="E28" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="20" t="s">
         <v>37</v>
       </c>
@@ -817,29 +830,33 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" s="12" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="19" t="n">
+      <c r="C30" s="21" t="n">
         <v>15</v>
       </c>
-      <c r="D30" s="19" t="n">
+      <c r="D30" s="21" t="n">
         <v>15</v>
       </c>
-      <c r="E30" s="19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="18" t="s">
+      <c r="E30" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19" t="n">
+      <c r="C31" s="21" t="n">
         <v>5</v>
       </c>
-      <c r="E31" s="19"/>
+      <c r="D31" s="21" t="n">
+        <v>5</v>
+      </c>
+      <c r="E31" s="21" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="23" t="s">
@@ -847,7 +864,7 @@
       </c>
       <c r="C32" s="24" t="n">
         <f aca="false">SUM(C6:C31)</f>
-        <v>437</v>
+        <v>484</v>
       </c>
       <c r="D32" s="24" t="n">
         <v>330</v>

</xml_diff>

<commit_message>
complete pagination and update evaluation protocol
</commit_message>
<xml_diff>
--- a/IssueTrackingSystem/docs/JS-Frameworks-Self-Evaluation-Protocol.xlsx
+++ b/IssueTrackingSystem/docs/JS-Frameworks-Self-Evaluation-Protocol.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
   <si>
     <t>JS-SPA-Self-Evaluation-Protocol</t>
   </si>
@@ -65,6 +65,9 @@
     <t>Numbers of Commits in GitHub</t>
   </si>
   <si>
+    <t>~278</t>
+  </si>
+  <si>
     <t>Basic Options (up to 150)</t>
   </si>
   <si>
@@ -95,7 +98,7 @@
     <t>Add Issue</t>
   </si>
   <si>
-    <t>Trqbva da go probvam kato admin ili lead</t>
+    <t>Admin or Lead</t>
   </si>
   <si>
     <t>Issue page</t>
@@ -215,12 +218,11 @@
     </font>
     <font>
       <b val="true"/>
-      <i val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -296,7 +298,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -357,6 +359,18 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -383,10 +397,6 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -474,10 +484,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:E32"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
+      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -559,7 +569,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="9" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>13</v>
@@ -572,8 +582,8 @@
       <c r="B9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="9" t="n">
-        <v>266</v>
+      <c r="C9" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>13</v>
@@ -584,7 +594,7 @@
     </row>
     <row r="10" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
@@ -592,7 +602,7 @@
     </row>
     <row r="11" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C11" s="14" t="n">
         <v>15</v>
@@ -601,12 +611,12 @@
         <v>20</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C12" s="14" t="n">
         <v>25</v>
@@ -615,12 +625,12 @@
         <v>30</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C13" s="14" t="n">
         <v>5</v>
@@ -629,12 +639,12 @@
         <v>5</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C14" s="14" t="n">
         <v>10</v>
@@ -643,12 +653,12 @@
         <v>10</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C15" s="14" t="n">
         <v>10</v>
@@ -657,12 +667,12 @@
         <v>10</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C16" s="14" t="n">
         <v>10</v>
@@ -671,36 +681,40 @@
         <v>10</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="E17" s="16"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="16" t="n">
-        <v>10</v>
-      </c>
-      <c r="D18" s="16" t="n">
-        <v>10</v>
-      </c>
-      <c r="E18" s="16" t="s">
+      <c r="D17" s="14" t="n">
+        <v>5</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" s="15" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="16" t="s">
         <v>26</v>
+      </c>
+      <c r="C18" s="17" t="n">
+        <v>10</v>
+      </c>
+      <c r="D18" s="17" t="n">
+        <v>10</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="19" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C19" s="14" t="n">
         <v>15</v>
@@ -708,21 +722,23 @@
       <c r="D19" s="14" t="n">
         <v>15</v>
       </c>
-      <c r="E19" s="14"/>
+      <c r="E19" s="14" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16" t="n">
-        <v>10</v>
-      </c>
-      <c r="E20" s="16"/>
+      <c r="B20" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19" t="n">
+        <v>10</v>
+      </c>
+      <c r="E20" s="19"/>
     </row>
     <row r="21" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C21" s="14" t="n">
         <v>10</v>
@@ -731,12 +747,12 @@
         <v>10</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C22" s="14" t="n">
         <v>5</v>
@@ -745,131 +761,136 @@
         <v>5</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16" t="n">
-        <v>10</v>
-      </c>
-      <c r="E23" s="16"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="14" t="n">
+        <v>10</v>
+      </c>
+      <c r="D23" s="14" t="n">
+        <v>10</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
+      <c r="B24" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="19" t="n">
+      <c r="B25" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="22" t="n">
         <v>20</v>
       </c>
-      <c r="D25" s="19" t="n">
+      <c r="D25" s="22" t="n">
         <v>20</v>
       </c>
-      <c r="E25" s="19" t="s">
-        <v>33</v>
+      <c r="E25" s="22" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="22" t="n">
+        <v>20</v>
+      </c>
+      <c r="D26" s="22" t="n">
+        <v>20</v>
+      </c>
+      <c r="E26" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="19" t="n">
-        <v>20</v>
-      </c>
-      <c r="D26" s="19" t="n">
-        <v>20</v>
-      </c>
-      <c r="E26" s="19" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
+      <c r="B27" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
     </row>
     <row r="28" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="21" t="n">
-        <v>10</v>
-      </c>
-      <c r="D28" s="21" t="n">
-        <v>10</v>
-      </c>
-      <c r="E28" s="21" t="s">
-        <v>18</v>
+      <c r="B28" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="24" t="n">
+        <v>10</v>
+      </c>
+      <c r="D28" s="24" t="n">
+        <v>10</v>
+      </c>
+      <c r="E28" s="24" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="29" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="C29" s="21" t="n">
-        <v>10</v>
-      </c>
-      <c r="D29" s="21" t="n">
-        <v>10</v>
-      </c>
-      <c r="E29" s="21" t="s">
-        <v>18</v>
+      <c r="B29" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="24" t="n">
+        <v>10</v>
+      </c>
+      <c r="D29" s="24" t="n">
+        <v>10</v>
+      </c>
+      <c r="E29" s="24" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="30" s="12" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="C30" s="21" t="n">
+      <c r="B30" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="24" t="n">
         <v>15</v>
       </c>
-      <c r="D30" s="21" t="n">
+      <c r="D30" s="24" t="n">
         <v>15</v>
       </c>
-      <c r="E30" s="21" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="31" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C31" s="21" t="n">
+      <c r="E30" s="24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="12"/>
+      <c r="B31" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="24" t="n">
         <v>5</v>
       </c>
-      <c r="D31" s="21" t="n">
+      <c r="D31" s="24" t="n">
         <v>5</v>
       </c>
-      <c r="E31" s="21" t="s">
-        <v>18</v>
+      <c r="E31" s="24" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="C32" s="24" t="n">
+      <c r="B32" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="26" t="n">
         <f aca="false">SUM(C6:C31)</f>
-        <v>484</v>
-      </c>
-      <c r="D32" s="24" t="n">
+        <v>232</v>
+      </c>
+      <c r="D32" s="26" t="n">
         <v>330</v>
       </c>
-      <c r="E32" s="23"/>
+      <c r="E32" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>